<commit_message>
version 1.0 forreal this time
</commit_message>
<xml_diff>
--- a/Tidskalkyle.xlsx
+++ b/Tidskalkyle.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11960" windowWidth="27500" xWindow="640" yWindow="600"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11960" windowWidth="27500" xWindow="640" yWindow="600"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Productcode:</t>
   </si>
@@ -38,10 +38,16 @@
     <t>Total Machining time:</t>
   </si>
   <si>
+    <t>164812</t>
+  </si>
+  <si>
+    <t>1:35:34</t>
+  </si>
+  <si>
     <t>156406</t>
   </si>
   <si>
-    <t>164812</t>
+    <t>1:2:52</t>
   </si>
 </sst>
 </file>
@@ -380,8 +386,8 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -432,9 +438,6 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" t="n">
-        <v>4266</v>
-      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="n"/>
@@ -460,10 +463,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -484,67 +487,18 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="n">
-        <v>3772</v>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="n">
-        <v>3772</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3772</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="n">
-        <v>3772</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="n">
-        <v>9506</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="n">
-        <v>9506</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="n">
-        <v>9506</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>9506</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2"/>
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
wonky gibbs is wonky
</commit_message>
<xml_diff>
--- a/Tidskalkyle.xlsx
+++ b/Tidskalkyle.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11955" windowWidth="27495" xWindow="645" yWindow="600"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11955" windowWidth="27495" xWindow="645" yWindow="600"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Productcode:</t>
   </si>
@@ -38,6 +38,9 @@
     <t>163767_M_Sylindrisk</t>
   </si>
   <si>
+    <t>102819_D_Bakside</t>
+  </si>
+  <si>
     <t>Total Machining time:</t>
   </si>
   <si>
@@ -57,6 +60,12 @@
   </si>
   <si>
     <t>1:35:34</t>
+  </si>
+  <si>
+    <t>102819</t>
+  </si>
+  <si>
+    <t>0:20:13</t>
   </si>
 </sst>
 </file>
@@ -395,11 +404,11 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="18.28515625"/>
     <col customWidth="1" max="2" min="2" width="13.42578125"/>
@@ -454,7 +463,12 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1" t="n"/>
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1213</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="n"/>
@@ -477,13 +491,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="12.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="20.42578125"/>
@@ -494,34 +508,42 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>